<commit_message>
Projet ---> CPC Couts
le programme permet de generer un cpc des couts à partir de la saisie d'un projet
</commit_message>
<xml_diff>
--- a/module classe projet/ModulePrincipal/References.xlsx
+++ b/module classe projet/ModulePrincipal/References.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{78E43248-3257-4DB2-A8F1-8F574E47B80E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{6684CFBA-BEA6-48B7-8F22-CD6A384456F1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20220" windowHeight="7275" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ref activite" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1544" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1542" uniqueCount="387">
   <si>
     <t>Hôtel</t>
   </si>
@@ -38052,8 +38052,8 @@
   </sheetPr>
   <dimension ref="A1:EK52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="P6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="P36" sqref="P36"/>
@@ -48189,10 +48189,10 @@
   <dimension ref="A2:AH33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="W2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I23" sqref="I23"/>
+      <selection pane="bottomRight" activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48599,9 +48599,7 @@
       <c r="J9" s="128"/>
       <c r="K9" s="128"/>
       <c r="L9" s="128"/>
-      <c r="M9" s="128" t="s">
-        <v>162</v>
-      </c>
+      <c r="M9" s="128"/>
       <c r="N9" s="128"/>
       <c r="O9" s="128"/>
       <c r="P9" s="128"/>
@@ -48847,9 +48845,7 @@
       <c r="L15" s="128"/>
       <c r="M15" s="128"/>
       <c r="N15" s="128"/>
-      <c r="O15" s="128" t="s">
-        <v>162</v>
-      </c>
+      <c r="O15" s="128"/>
       <c r="P15" s="128"/>
       <c r="Q15" s="128"/>
       <c r="R15" s="128"/>
@@ -49237,8 +49233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3F66C91-4BF6-4937-8467-CCC69562F4F2}">
   <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>